<commit_message>
terceira versão quase finalizada
</commit_message>
<xml_diff>
--- a/Calculo da equação.xlsx
+++ b/Calculo da equação.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\Tarefas Engenharia de Software\2° Semestre\Algoritimos e Progamação Estruturada\Trabalho de Algoritimo N1\Trabalho N1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3648B0-8F69-4191-AE99-DCE06F51CFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D88435-31BD-4E75-AB65-9B078B89908C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{E62F1AE4-2A70-4F43-B51C-67E41213893B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E62F1AE4-2A70-4F43-B51C-67E41213893B}"/>
   </bookViews>
   <sheets>
     <sheet name="1° Caso de Teste" sheetId="1" r:id="rId1"/>
@@ -227,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -300,20 +300,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -373,12 +364,6 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -390,6 +375,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -793,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28ECF17-F12D-4430-A5DA-09223A791C2F}">
   <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView zoomScale="113" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -848,10 +842,10 @@
       <c r="G7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="25"/>
+      <c r="I7" s="23"/>
       <c r="J7" s="11" t="s">
         <v>26</v>
       </c>
@@ -873,16 +867,17 @@
       <c r="P7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="Q7" s="10" t="s">
+      <c r="Q7" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="S7" s="22" t="s">
+      <c r="R7" s="26"/>
+      <c r="S7" s="10" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="D8" s="26">
+      <c r="D8" s="24">
         <v>0</v>
       </c>
       <c r="E8" s="7">
@@ -937,14 +932,14 @@
         <f>Q8+F8</f>
         <v>155.69090358436199</v>
       </c>
-      <c r="S8" s="1" t="str">
+      <c r="S8" s="3" t="str">
         <f>CHAR(F8)</f>
         <v>V</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="D9" s="26"/>
+      <c r="D9" s="24"/>
       <c r="E9" s="7" t="s">
         <v>0</v>
       </c>
@@ -998,14 +993,14 @@
         <f>Q9+F9</f>
         <v>113.99977166873597</v>
       </c>
-      <c r="S9" s="1" t="str">
+      <c r="S9" s="3" t="str">
         <f>CHAR(F9)</f>
         <v>o</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="D10" s="26"/>
+      <c r="D10" s="24"/>
       <c r="E10" s="7">
         <v>63</v>
       </c>
@@ -1059,14 +1054,14 @@
         <f t="shared" ref="R10:R58" si="9">Q10+F10</f>
         <v>70.486602108493983</v>
       </c>
-      <c r="S10" s="1" t="str">
+      <c r="S10" s="3" t="str">
         <f t="shared" ref="S10:S58" si="10">CHAR(F10)</f>
         <v>c</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="D11" s="26"/>
+      <c r="D11" s="24"/>
       <c r="E11" s="7">
         <v>88</v>
       </c>
@@ -1120,14 +1115,14 @@
         <f t="shared" si="9"/>
         <v>99.234034423807941</v>
       </c>
-      <c r="S11" s="1" t="str">
+      <c r="S11" s="3" t="str">
         <f t="shared" si="10"/>
         <v>ˆ</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="D12" s="26"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="7">
         <v>73</v>
       </c>
@@ -1181,14 +1176,14 @@
         <f t="shared" si="9"/>
         <v>84.108378281249941</v>
       </c>
-      <c r="S12" s="1" t="str">
+      <c r="S12" s="3" t="str">
         <f t="shared" si="10"/>
         <v>s</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="D13" s="26"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="7">
         <v>20</v>
       </c>
@@ -1242,14 +1237,14 @@
         <f t="shared" si="9"/>
         <v>14.315214168831943</v>
       </c>
-      <c r="S13" s="1" t="str">
+      <c r="S13" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="D14" s="26"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="7">
         <v>73</v>
       </c>
@@ -1303,13 +1298,14 @@
         <f t="shared" si="9"/>
         <v>112.99943919296594</v>
       </c>
-      <c r="S14" s="1" t="str">
+      <c r="S14" s="3" t="str">
         <f t="shared" si="10"/>
         <v>s</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
+      <c r="D15" s="27"/>
       <c r="E15" s="7" t="s">
         <v>1</v>
       </c>
@@ -1363,13 +1359,14 @@
         <f t="shared" si="9"/>
         <v>210.88763092582371</v>
       </c>
-      <c r="S15" s="1" t="str">
+      <c r="S15" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Æ</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
+      <c r="D16" s="27"/>
       <c r="E16" s="7" t="s">
         <v>0</v>
       </c>
@@ -1381,8 +1378,8 @@
         <f t="shared" si="11"/>
         <v>9</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
       <c r="J16" s="12">
         <f t="shared" si="1"/>
         <v>-1147.3630000000003</v>
@@ -1419,13 +1416,14 @@
         <f t="shared" si="9"/>
         <v>135.97060223157703</v>
       </c>
-      <c r="S16" s="1" t="str">
+      <c r="S16" s="3" t="str">
         <f t="shared" si="10"/>
         <v>o</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="7">
         <v>20</v>
       </c>
@@ -1437,8 +1435,8 @@
         <f t="shared" si="11"/>
         <v>10</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
       <c r="J17" s="12">
         <f t="shared" si="1"/>
         <v>-1295.5980000000002</v>
@@ -1475,13 +1473,14 @@
         <f t="shared" si="9"/>
         <v>65.224019999999797</v>
       </c>
-      <c r="S17" s="1" t="str">
+      <c r="S17" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
+      <c r="D18" s="27"/>
       <c r="E18" s="7">
         <v>76</v>
       </c>
@@ -1493,8 +1492,8 @@
         <f t="shared" si="11"/>
         <v>11</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
       <c r="J18" s="12">
         <f t="shared" si="1"/>
         <v>-1443.8330000000001</v>
@@ -1531,13 +1530,14 @@
         <f t="shared" si="9"/>
         <v>155.36496071590105</v>
       </c>
-      <c r="S18" s="1" t="str">
+      <c r="S18" s="3" t="str">
         <f t="shared" si="10"/>
         <v>v</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
+      <c r="D19" s="27"/>
       <c r="E19" s="7">
         <v>65</v>
       </c>
@@ -1549,8 +1549,8 @@
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
       <c r="J19" s="12">
         <f t="shared" si="1"/>
         <v>-1592.0680000000002</v>
@@ -1587,13 +1587,14 @@
         <f t="shared" si="9"/>
         <v>138.64227579289627</v>
       </c>
-      <c r="S19" s="1" t="str">
+      <c r="S19" s="3" t="str">
         <f t="shared" si="10"/>
         <v>e</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
+      <c r="D20" s="27"/>
       <c r="E20" s="7" t="s">
         <v>2</v>
       </c>
@@ -1605,8 +1606,8 @@
         <f t="shared" si="11"/>
         <v>13</v>
       </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
       <c r="J20" s="12">
         <f t="shared" si="1"/>
         <v>-1740.3030000000003</v>
@@ -1643,13 +1644,14 @@
         <f t="shared" si="9"/>
         <v>144.65863959995295</v>
       </c>
-      <c r="S20" s="1" t="str">
+      <c r="S20" s="3" t="str">
         <f t="shared" si="10"/>
         <v>n</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
+      <c r="D21" s="27"/>
       <c r="E21" s="7">
         <v>63</v>
       </c>
@@ -1661,8 +1663,8 @@
         <f t="shared" si="11"/>
         <v>14</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
       <c r="J21" s="12">
         <f t="shared" si="1"/>
         <v>-1888.538</v>
@@ -1699,13 +1701,14 @@
         <f t="shared" si="9"/>
         <v>128.2221531092473</v>
       </c>
-      <c r="S21" s="1" t="str">
+      <c r="S21" s="3" t="str">
         <f t="shared" si="10"/>
         <v>c</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
+      <c r="D22" s="27"/>
       <c r="E22" s="7">
         <v>65</v>
       </c>
@@ -1717,6 +1720,8 @@
         <f t="shared" si="11"/>
         <v>15</v>
       </c>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
       <c r="J22" s="12">
         <f t="shared" si="1"/>
         <v>-2036.7730000000001</v>
@@ -1753,13 +1758,14 @@
         <f t="shared" si="9"/>
         <v>123.22537609374966</v>
       </c>
-      <c r="S22" s="1" t="str">
+      <c r="S22" s="3" t="str">
         <f t="shared" si="10"/>
         <v>e</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
+      <c r="D23" s="27"/>
       <c r="E23" s="7">
         <v>64</v>
       </c>
@@ -1771,6 +1777,8 @@
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
       <c r="J23" s="12">
         <f t="shared" si="1"/>
         <v>-2185.0080000000003</v>
@@ -1807,13 +1815,14 @@
         <f t="shared" si="9"/>
         <v>114.54966080307128</v>
       </c>
-      <c r="S23" s="1" t="str">
+      <c r="S23" s="3" t="str">
         <f t="shared" si="10"/>
         <v>d</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
+      <c r="D24" s="27"/>
       <c r="E24" s="7" t="s">
         <v>0</v>
       </c>
@@ -1825,6 +1834,8 @@
         <f t="shared" si="11"/>
         <v>17</v>
       </c>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
       <c r="J24" s="12">
         <f t="shared" si="1"/>
         <v>-2333.2430000000004</v>
@@ -1861,13 +1872,14 @@
         <f t="shared" si="9"/>
         <v>117.99266004602322</v>
       </c>
-      <c r="S24" s="1" t="str">
+      <c r="S24" s="3" t="str">
         <f t="shared" si="10"/>
         <v>o</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
+      <c r="D25" s="27"/>
       <c r="E25" s="7">
         <v>86</v>
       </c>
@@ -1879,6 +1891,8 @@
         <f t="shared" si="11"/>
         <v>18</v>
       </c>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
       <c r="J25" s="12">
         <f t="shared" si="1"/>
         <v>-2481.4780000000005</v>
@@ -1915,13 +1929,14 @@
         <f t="shared" si="9"/>
         <v>134.21688260837772</v>
       </c>
-      <c r="S25" s="1" t="str">
+      <c r="S25" s="3" t="str">
         <f t="shared" si="10"/>
         <v>†</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
+      <c r="D26" s="27"/>
       <c r="E26" s="7">
         <v>72</v>
       </c>
@@ -1933,6 +1948,8 @@
         <f t="shared" si="11"/>
         <v>19</v>
       </c>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
       <c r="J26" s="12">
         <f t="shared" si="1"/>
         <v>-2629.7130000000002</v>
@@ -1969,13 +1986,14 @@
         <f t="shared" si="9"/>
         <v>108.71716893431579</v>
       </c>
-      <c r="S26" s="1" t="str">
+      <c r="S26" s="3" t="str">
         <f t="shared" si="10"/>
         <v>r</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
+      <c r="D27" s="27"/>
       <c r="E27" s="7">
         <v>65</v>
       </c>
@@ -1987,6 +2005,8 @@
         <f t="shared" si="11"/>
         <v>20</v>
       </c>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
       <c r="J27" s="12">
         <f t="shared" si="1"/>
         <v>-2777.9480000000003</v>
@@ -2023,13 +2043,14 @@
         <f t="shared" si="9"/>
         <v>91.804959999998459</v>
       </c>
-      <c r="S27" s="1" t="str">
+      <c r="S27" s="3" t="str">
         <f t="shared" si="10"/>
         <v>e</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
+      <c r="D28" s="27"/>
       <c r="E28" s="7">
         <v>73</v>
       </c>
@@ -2041,6 +2062,8 @@
         <f t="shared" si="11"/>
         <v>21</v>
       </c>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
       <c r="J28" s="12">
         <f t="shared" si="1"/>
         <v>-2926.1830000000004</v>
@@ -2077,13 +2100,14 @@
         <f t="shared" si="9"/>
         <v>103.60723230783697</v>
       </c>
-      <c r="S28" s="1" t="str">
+      <c r="S28" s="3" t="str">
         <f t="shared" si="10"/>
         <v>s</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
+      <c r="D29" s="27"/>
       <c r="E29" s="7" t="s">
         <v>3</v>
       </c>
@@ -2095,6 +2119,8 @@
         <f t="shared" si="11"/>
         <v>22</v>
       </c>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
       <c r="J29" s="12">
         <f t="shared" si="1"/>
         <v>-3074.4180000000001</v>
@@ -2131,13 +2157,14 @@
         <f t="shared" si="9"/>
         <v>32.077971929850264</v>
       </c>
-      <c r="S29" s="1" t="str">
+      <c r="S29" s="3" t="str">
         <f t="shared" si="10"/>
         <v>,</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
+      <c r="D30" s="27"/>
       <c r="E30" s="7">
         <v>20</v>
       </c>
@@ -2149,6 +2176,8 @@
         <f t="shared" si="11"/>
         <v>23</v>
       </c>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
       <c r="J30" s="12">
         <f t="shared" si="1"/>
         <v>-3222.6530000000002</v>
@@ -2185,13 +2214,14 @@
         <f t="shared" si="9"/>
         <v>21.020060528607246</v>
       </c>
-      <c r="S30" s="1" t="str">
+      <c r="S30" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
+      <c r="D31" s="27"/>
       <c r="E31" s="7">
         <v>76</v>
       </c>
@@ -2203,6 +2233,8 @@
         <f t="shared" si="11"/>
         <v>24</v>
       </c>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
       <c r="J31" s="12">
         <f t="shared" si="1"/>
         <v>-3370.8880000000004</v>
@@ -2239,13 +2271,14 @@
         <f t="shared" si="9"/>
         <v>109.11544628429647</v>
       </c>
-      <c r="S31" s="1" t="str">
+      <c r="S31" s="3" t="str">
         <f t="shared" si="10"/>
         <v>v</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
+      <c r="D32" s="27"/>
       <c r="E32" s="7" t="s">
         <v>0</v>
       </c>
@@ -2257,6 +2290,8 @@
         <f t="shared" si="11"/>
         <v>25</v>
       </c>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
       <c r="J32" s="12">
         <f t="shared" si="1"/>
         <v>-3519.1230000000005</v>
@@ -2293,13 +2328,14 @@
         <f t="shared" si="9"/>
         <v>104.96147265625086</v>
       </c>
-      <c r="S32" s="1" t="str">
+      <c r="S32" s="3" t="str">
         <f t="shared" si="10"/>
         <v>o</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
+      <c r="D33" s="27"/>
       <c r="E33" s="7">
         <v>63</v>
       </c>
@@ -2311,6 +2347,8 @@
         <f t="shared" si="11"/>
         <v>26</v>
       </c>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
       <c r="J33" s="12">
         <f t="shared" si="1"/>
         <v>-3667.3580000000006</v>
@@ -2347,13 +2385,14 @@
         <f t="shared" si="9"/>
         <v>96.111237907696704</v>
       </c>
-      <c r="S33" s="1" t="str">
+      <c r="S33" s="3" t="str">
         <f t="shared" si="10"/>
         <v>c</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
+      <c r="D34" s="27"/>
       <c r="E34" s="7" t="s">
         <v>4</v>
       </c>
@@ -2365,6 +2404,8 @@
         <f t="shared" si="11"/>
         <v>27</v>
       </c>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
       <c r="J34" s="12">
         <f t="shared" si="1"/>
         <v>-3815.5930000000003</v>
@@ -2401,13 +2442,14 @@
         <f t="shared" si="9"/>
         <v>195.11585832187666</v>
       </c>
-      <c r="S34" s="1" t="str">
+      <c r="S34" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Ã</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
+      <c r="D35" s="27"/>
       <c r="E35" s="7">
         <v>88</v>
       </c>
@@ -2419,6 +2461,8 @@
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
       <c r="J35" s="12">
         <f t="shared" si="1"/>
         <v>-3963.828</v>
@@ -2455,13 +2499,14 @@
         <f t="shared" si="9"/>
         <v>138.566508038145</v>
       </c>
-      <c r="S35" s="1" t="str">
+      <c r="S35" s="3" t="str">
         <f t="shared" si="10"/>
         <v>ˆ</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
+      <c r="D36" s="27"/>
       <c r="E36" s="7">
         <v>73</v>
       </c>
@@ -2473,6 +2518,8 @@
         <f t="shared" si="11"/>
         <v>29</v>
       </c>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
       <c r="J36" s="12">
         <f t="shared" si="1"/>
         <v>-4112.0630000000001</v>
@@ -2509,13 +2556,14 @@
         <f t="shared" si="9"/>
         <v>119.13410843666043</v>
       </c>
-      <c r="S36" s="1" t="str">
+      <c r="S36" s="3" t="str">
         <f t="shared" si="10"/>
         <v>s</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
+      <c r="D37" s="27"/>
       <c r="E37" s="7">
         <v>20</v>
       </c>
@@ -2527,6 +2575,8 @@
         <f t="shared" si="11"/>
         <v>30</v>
       </c>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
       <c r="J37" s="12">
         <f t="shared" si="1"/>
         <v>-4260.2979999999998</v>
@@ -2563,13 +2613,14 @@
         <f t="shared" si="9"/>
         <v>36.604540000005727</v>
       </c>
-      <c r="S37" s="1" t="str">
+      <c r="S37" s="3" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
+      <c r="D38" s="27"/>
       <c r="E38" s="7">
         <v>63</v>
       </c>
@@ -2581,6 +2632,8 @@
         <f t="shared" si="11"/>
         <v>31</v>
       </c>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
       <c r="J38" s="12">
         <f t="shared" si="1"/>
         <v>-4408.5330000000004</v>
@@ -2617,13 +2670,14 @@
         <f t="shared" si="9"/>
         <v>102.90724958017381</v>
       </c>
-      <c r="S38" s="1" t="str">
+      <c r="S38" s="3" t="str">
         <f t="shared" si="10"/>
         <v>c</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
+      <c r="D39" s="27"/>
       <c r="E39" s="7" t="s">
         <v>0</v>
       </c>
@@ -2635,6 +2689,8 @@
         <f t="shared" si="11"/>
         <v>32</v>
       </c>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
       <c r="J39" s="12">
         <f t="shared" si="1"/>
         <v>-4556.768</v>
@@ -2671,13 +2727,14 @@
         <f t="shared" si="9"/>
         <v>113.13512599960814</v>
       </c>
-      <c r="S39" s="1" t="str">
+      <c r="S39" s="3" t="str">
         <f t="shared" si="10"/>
         <v>o</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
+      <c r="D40" s="27"/>
       <c r="E40" s="7" t="s">
         <v>5</v>
       </c>
@@ -2689,6 +2746,8 @@
         <f t="shared" si="11"/>
         <v>33</v>
       </c>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
       <c r="J40" s="12">
         <f t="shared" si="1"/>
         <v>-4705.0029999999997</v>
@@ -2725,13 +2784,14 @@
         <f t="shared" si="9"/>
         <v>189.55351691446776</v>
       </c>
-      <c r="S40" s="1" t="str">
+      <c r="S40" s="3" t="str">
         <f t="shared" si="10"/>
         <v>¾</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
+      <c r="D41" s="27"/>
       <c r="E41" s="7" t="s">
         <v>2</v>
       </c>
@@ -2743,6 +2803,8 @@
         <f t="shared" si="11"/>
         <v>34</v>
       </c>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
       <c r="J41" s="12">
         <f t="shared" si="1"/>
         <v>-4853.2380000000003</v>
@@ -2779,13 +2841,14 @@
         <f t="shared" si="9"/>
         <v>106.59625986890023</v>
       </c>
-      <c r="S41" s="1" t="str">
+      <c r="S41" s="3" t="str">
         <f t="shared" si="10"/>
         <v>n</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
+      <c r="D42" s="27"/>
       <c r="E42" s="7">
         <v>73</v>
       </c>
@@ -2797,6 +2860,8 @@
         <f t="shared" si="11"/>
         <v>35</v>
       </c>
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
       <c r="J42" s="12">
         <f t="shared" si="1"/>
         <v>-5001.473</v>
@@ -2833,13 +2898,14 @@
         <f t="shared" si="9"/>
         <v>108.84660046876525</v>
       </c>
-      <c r="S42" s="1" t="str">
+      <c r="S42" s="3" t="str">
         <f t="shared" si="10"/>
         <v>s</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
+      <c r="D43" s="27"/>
       <c r="E43" s="7">
         <v>65</v>
       </c>
@@ -2851,6 +2917,8 @@
         <f t="shared" si="11"/>
         <v>36</v>
       </c>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
       <c r="J43" s="12">
         <f t="shared" si="1"/>
         <v>-5149.7080000000005</v>
@@ -2887,13 +2955,14 @@
         <f t="shared" si="9"/>
         <v>93.000870602692885</v>
       </c>
-      <c r="S43" s="1" t="str">
+      <c r="S43" s="3" t="str">
         <f t="shared" si="10"/>
         <v>e</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
+      <c r="D44" s="27"/>
       <c r="E44" s="7">
         <v>67</v>
       </c>
@@ -2905,6 +2974,8 @@
         <f t="shared" si="11"/>
         <v>37</v>
       </c>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
       <c r="J44" s="12">
         <f t="shared" si="1"/>
         <v>-5297.9430000000002</v>
@@ -2941,13 +3012,14 @@
         <f t="shared" si="9"/>
         <v>94.812799640516459</v>
       </c>
-      <c r="S44" s="1" t="str">
+      <c r="S44" s="3" t="str">
         <f t="shared" si="10"/>
         <v>g</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
+      <c r="D45" s="27"/>
       <c r="E45" s="7">
         <v>75</v>
       </c>
@@ -2959,6 +3031,8 @@
         <f t="shared" si="11"/>
         <v>38</v>
       </c>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
       <c r="J45" s="12">
         <f t="shared" si="1"/>
         <v>-5446.1779999999999</v>
@@ -2995,13 +3069,14 @@
         <f t="shared" si="9"/>
         <v>111.01633153508737</v>
       </c>
-      <c r="S45" s="1" t="str">
+      <c r="S45" s="3" t="str">
         <f t="shared" si="10"/>
         <v>u</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
+      <c r="D46" s="27"/>
       <c r="E46" s="7">
         <v>65</v>
       </c>
@@ -3013,6 +3088,8 @@
         <f t="shared" si="11"/>
         <v>39</v>
       </c>
+      <c r="H46" s="27"/>
+      <c r="I46" s="27"/>
       <c r="J46" s="12">
         <f t="shared" si="1"/>
         <v>-5594.4130000000005</v>
@@ -3049,13 +3126,14 @@
         <f t="shared" si="9"/>
         <v>100.22482075856533</v>
       </c>
-      <c r="S46" s="1" t="str">
+      <c r="S46" s="3" t="str">
         <f t="shared" si="10"/>
         <v>e</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
+      <c r="D47" s="27"/>
       <c r="E47" s="7" t="s">
         <v>6</v>
       </c>
@@ -3067,6 +3145,8 @@
         <f t="shared" si="11"/>
         <v>40</v>
       </c>
+      <c r="H47" s="27"/>
+      <c r="I47" s="27"/>
       <c r="J47" s="12">
         <f t="shared" si="1"/>
         <v>-5742.6480000000001</v>
@@ -3103,13 +3183,14 @@
         <f t="shared" si="9"/>
         <v>116.80448000003526</v>
       </c>
-      <c r="S47" s="1" t="str">
+      <c r="S47" s="3" t="str">
         <f t="shared" si="10"/>
         <v>m</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
+      <c r="D48" s="27"/>
       <c r="E48" s="7" t="s">
         <v>7</v>
       </c>
@@ -3121,6 +3202,8 @@
         <f t="shared" si="11"/>
         <v>41</v>
       </c>
+      <c r="H48" s="27"/>
+      <c r="I48" s="27"/>
       <c r="J48" s="12">
         <f t="shared" si="1"/>
         <v>-5890.8829999999998</v>
@@ -3157,13 +3240,14 @@
         <f t="shared" si="9"/>
         <v>65.719952552986797</v>
       </c>
-      <c r="S48" s="1" t="str">
+      <c r="S48" s="3" t="str">
         <f t="shared" si="10"/>
         <v>.</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
+      <c r="D49" s="27"/>
       <c r="E49" s="7">
         <v>0</v>
       </c>
@@ -3175,6 +3259,8 @@
         <f t="shared" si="11"/>
         <v>42</v>
       </c>
+      <c r="H49" s="27"/>
+      <c r="I49" s="27"/>
       <c r="J49" s="12">
         <f t="shared" si="1"/>
         <v>-6039.1180000000004</v>
@@ -3211,13 +3297,14 @@
         <f t="shared" si="9"/>
         <v>34.349882322130725</v>
       </c>
-      <c r="S49" s="1" t="e">
+      <c r="S49" s="3" t="e">
         <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
+      <c r="D50" s="27"/>
       <c r="E50" s="15" t="s">
         <v>8</v>
       </c>
@@ -3229,8 +3316,8 @@
         <f t="shared" si="11"/>
         <v>43</v>
       </c>
-      <c r="H50" s="17"/>
-      <c r="I50" s="17"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="27"/>
       <c r="J50" s="18">
         <f t="shared" si="1"/>
         <v>-6187.3530000000001</v>
@@ -3267,13 +3354,14 @@
         <f t="shared" si="9"/>
         <v>95.270354377556941</v>
       </c>
-      <c r="S50" s="1" t="str">
+      <c r="S50" s="3" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
+      <c r="D51" s="27"/>
       <c r="E51" s="7" t="s">
         <v>1</v>
       </c>
@@ -3285,6 +3373,8 @@
         <f t="shared" si="11"/>
         <v>44</v>
       </c>
+      <c r="H51" s="27"/>
+      <c r="I51" s="27"/>
       <c r="J51" s="12">
         <f t="shared" si="1"/>
         <v>-6335.5879999999997</v>
@@ -3321,12 +3411,13 @@
         <f t="shared" si="9"/>
         <v>263.00407898309641</v>
       </c>
-      <c r="S51" s="1" t="str">
+      <c r="S51" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Æ</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D52" s="27"/>
       <c r="E52" s="7" t="s">
         <v>9</v>
       </c>
@@ -3338,6 +3429,8 @@
         <f t="shared" si="11"/>
         <v>45</v>
       </c>
+      <c r="H52" s="27"/>
+      <c r="I52" s="27"/>
       <c r="J52" s="12">
         <f t="shared" si="1"/>
         <v>-6483.8230000000003</v>
@@ -3374,12 +3467,13 @@
         <f t="shared" si="9"/>
         <v>275.73319203127176</v>
       </c>
-      <c r="S52" s="1" t="str">
+      <c r="S52" s="3" t="str">
         <f t="shared" si="10"/>
         <v>É</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D53" s="27"/>
       <c r="E53" s="7">
         <v>21</v>
       </c>
@@ -3391,6 +3485,8 @@
         <f t="shared" si="11"/>
         <v>46</v>
       </c>
+      <c r="H53" s="27"/>
+      <c r="I53" s="27"/>
       <c r="J53" s="12">
         <f t="shared" si="1"/>
         <v>-6632.058</v>
@@ -3427,12 +3523,13 @@
         <f t="shared" si="9"/>
         <v>106.97354480810463</v>
       </c>
-      <c r="S53" s="1" t="str">
+      <c r="S53" s="3" t="str">
         <f t="shared" si="10"/>
         <v>!</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D54" s="27"/>
       <c r="E54" s="7" t="s">
         <v>10</v>
       </c>
@@ -3444,6 +3541,8 @@
         <f t="shared" si="11"/>
         <v>47</v>
       </c>
+      <c r="H54" s="27"/>
+      <c r="I54" s="27"/>
       <c r="J54" s="12">
         <f t="shared" si="1"/>
         <v>-6780.2930000000006</v>
@@ -3480,12 +3579,13 @@
         <f t="shared" si="9"/>
         <v>238.20835602207808</v>
       </c>
-      <c r="S54" s="1" t="str">
+      <c r="S54" s="3" t="str">
         <f t="shared" si="10"/>
         <v>·</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D55" s="27"/>
       <c r="E55" s="7" t="s">
         <v>11</v>
       </c>
@@ -3497,6 +3597,8 @@
         <f t="shared" si="11"/>
         <v>48</v>
       </c>
+      <c r="H55" s="27"/>
+      <c r="I55" s="27"/>
       <c r="J55" s="12">
         <f t="shared" si="1"/>
         <v>-6928.5280000000002</v>
@@ -3533,12 +3635,13 @@
         <f t="shared" si="9"/>
         <v>192.47909901948879</v>
       </c>
-      <c r="S55" s="1" t="str">
+      <c r="S55" s="3" t="str">
         <f t="shared" si="10"/>
         <v>¸</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D56" s="27"/>
       <c r="E56" s="7" t="s">
         <v>12</v>
       </c>
@@ -3550,6 +3653,8 @@
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
+      <c r="H56" s="27"/>
+      <c r="I56" s="27"/>
       <c r="J56" s="12">
         <f t="shared" si="1"/>
         <v>-7076.7629999999999</v>
@@ -3586,12 +3691,13 @@
         <f t="shared" si="9"/>
         <v>47.93149712018203</v>
       </c>
-      <c r="S56" s="1" t="str">
+      <c r="S56" s="3" t="str">
         <f t="shared" si="10"/>
         <v></v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D57" s="27"/>
       <c r="E57" s="7" t="s">
         <v>13</v>
       </c>
@@ -3603,6 +3709,8 @@
         <f t="shared" si="11"/>
         <v>50</v>
       </c>
+      <c r="H57" s="27"/>
+      <c r="I57" s="27"/>
       <c r="J57" s="12">
         <f t="shared" si="1"/>
         <v>-7224.9980000000005</v>
@@ -3639,12 +3747,13 @@
         <f t="shared" si="9"/>
         <v>-16.685499999963213</v>
       </c>
-      <c r="S57" s="1" t="str">
+      <c r="S57" s="3" t="str">
         <f t="shared" si="10"/>
         <v>Ï</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D58" s="27"/>
       <c r="E58" s="7"/>
       <c r="F58" s="2">
         <f t="shared" si="12"/>
@@ -3654,6 +3763,8 @@
         <f t="shared" si="11"/>
         <v>51</v>
       </c>
+      <c r="H58" s="27"/>
+      <c r="I58" s="27"/>
       <c r="J58" s="12">
         <f t="shared" si="1"/>
         <v>-7373.2330000000002</v>
@@ -3690,15 +3801,18 @@
         <f t="shared" si="9"/>
         <v>-445.5698859540862</v>
       </c>
-      <c r="S58" s="1" t="e">
+      <c r="S58" s="3" t="e">
         <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="D8:D14"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="H16:I58"/>
+    <mergeCell ref="D15:D58"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F7:F58">
@@ -3764,10 +3878,10 @@
       <c r="G7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="25"/>
+      <c r="I7" s="23"/>
       <c r="J7" s="11" t="s">
         <v>26</v>
       </c>
@@ -3800,7 +3914,7 @@
       </c>
     </row>
     <row r="8" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D8" s="26">
+      <c r="D8" s="24">
         <v>3</v>
       </c>
       <c r="E8" s="7">
@@ -3851,7 +3965,7 @@
         <f>J8+K8+L8+M8+N8+O8+P8</f>
         <v>72.69090358436199</v>
       </c>
-      <c r="R8" s="23">
+      <c r="R8" s="21">
         <f>Q8+F8</f>
         <v>156.69090358436199</v>
       </c>
@@ -3861,7 +3975,7 @@
       </c>
     </row>
     <row r="9" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D9" s="26"/>
+      <c r="D9" s="24"/>
       <c r="E9" s="7">
         <v>65</v>
       </c>
@@ -3911,7 +4025,7 @@
         <f t="shared" ref="Q9:Q58" si="8">J9+K9+L9+M9+N9+O9+P9</f>
         <v>8.9997716687359777</v>
       </c>
-      <c r="R9" s="23">
+      <c r="R9" s="21">
         <f>Q9+F9</f>
         <v>109.99977166873597</v>
       </c>
@@ -3921,7 +4035,7 @@
       </c>
     </row>
     <row r="10" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D10" s="26"/>
+      <c r="D10" s="24"/>
       <c r="E10" s="7">
         <v>63</v>
       </c>
@@ -3971,7 +4085,7 @@
         <f t="shared" si="8"/>
         <v>-19.513397891506013</v>
       </c>
-      <c r="R10" s="23">
+      <c r="R10" s="21">
         <f t="shared" ref="R10:R58" si="9">Q10+F10</f>
         <v>79.486602108493983</v>
       </c>
@@ -3981,7 +4095,7 @@
       </c>
     </row>
     <row r="11" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D11" s="26"/>
+      <c r="D11" s="24"/>
       <c r="E11" s="7" t="s">
         <v>2</v>
       </c>
@@ -4031,7 +4145,7 @@
         <f t="shared" si="8"/>
         <v>-24.765965576192066</v>
       </c>
-      <c r="R11" s="23">
+      <c r="R11" s="21">
         <f t="shared" si="9"/>
         <v>85.234034423807941</v>
       </c>
@@ -4041,7 +4155,7 @@
       </c>
     </row>
     <row r="12" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D12" s="26"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="7" t="s">
         <v>0</v>
       </c>
@@ -4091,7 +4205,7 @@
         <f t="shared" si="8"/>
         <v>-15.891621718750054</v>
       </c>
-      <c r="R12" s="23">
+      <c r="R12" s="21">
         <f t="shared" si="9"/>
         <v>95.108378281249941</v>
       </c>
@@ -4101,7 +4215,7 @@
       </c>
     </row>
     <row r="13" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D13" s="26"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="7">
         <v>33</v>
       </c>
@@ -4151,7 +4265,7 @@
         <f t="shared" si="8"/>
         <v>0.31521416883194397</v>
       </c>
-      <c r="R13" s="23">
+      <c r="R13" s="21">
         <f t="shared" si="9"/>
         <v>51.315214168831943</v>
       </c>
@@ -4161,7 +4275,7 @@
       </c>
     </row>
     <row r="14" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D14" s="26"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="7" t="s">
         <v>37</v>
       </c>
@@ -4211,7 +4325,7 @@
         <f t="shared" si="8"/>
         <v>18.999439192965934</v>
       </c>
-      <c r="R14" s="23">
+      <c r="R14" s="21">
         <f t="shared" si="9"/>
         <v>126.99943919296594</v>
       </c>
@@ -4270,7 +4384,7 @@
         <f t="shared" si="8"/>
         <v>36.887630925823714</v>
       </c>
-      <c r="R15" s="23">
+      <c r="R15" s="21">
         <f t="shared" si="9"/>
         <v>147.88763092582371</v>
       </c>
@@ -4325,7 +4439,7 @@
         <f t="shared" si="8"/>
         <v>51.970602231577047</v>
       </c>
-      <c r="R16" s="23">
+      <c r="R16" s="21">
         <f t="shared" si="9"/>
         <v>154.97060223157706</v>
       </c>
@@ -4380,7 +4494,7 @@
         <f t="shared" si="8"/>
         <v>63.224019999999804</v>
       </c>
-      <c r="R17" s="23">
+      <c r="R17" s="21">
         <f t="shared" si="9"/>
         <v>168.2240199999998</v>
       </c>
@@ -4435,7 +4549,7 @@
         <f t="shared" si="8"/>
         <v>70.364960715901049</v>
       </c>
-      <c r="R18" s="23">
+      <c r="R18" s="21">
         <f t="shared" si="9"/>
         <v>167.36496071590105</v>
       </c>
@@ -4490,7 +4604,7 @@
         <f t="shared" si="8"/>
         <v>73.642275792896285</v>
       </c>
-      <c r="R19" s="23">
+      <c r="R19" s="21">
         <f t="shared" si="9"/>
         <v>105.64227579289629</v>
       </c>
@@ -4545,7 +4659,7 @@
         <f t="shared" si="8"/>
         <v>73.65863959995248</v>
       </c>
-      <c r="R20" s="23">
+      <c r="R20" s="21">
         <f t="shared" si="9"/>
         <v>173.65863959995249</v>
       </c>
@@ -4600,7 +4714,7 @@
         <f t="shared" si="8"/>
         <v>71.222153109247301</v>
       </c>
-      <c r="R21" s="23">
+      <c r="R21" s="21">
         <f t="shared" si="9"/>
         <v>168.2221531092473</v>
       </c>
@@ -4653,7 +4767,7 @@
         <f t="shared" si="8"/>
         <v>67.225376093749659</v>
       </c>
-      <c r="R22" s="23">
+      <c r="R22" s="21">
         <f t="shared" si="9"/>
         <v>99.225376093749659</v>
       </c>
@@ -4706,7 +4820,7 @@
         <f t="shared" si="8"/>
         <v>62.549660803071276</v>
       </c>
-      <c r="R23" s="23">
+      <c r="R23" s="21">
         <f t="shared" si="9"/>
         <v>135.54966080307128</v>
       </c>
@@ -4759,7 +4873,7 @@
         <f t="shared" si="8"/>
         <v>57.992660046023218</v>
       </c>
-      <c r="R24" s="23">
+      <c r="R24" s="21">
         <f t="shared" si="9"/>
         <v>167.99266004602322</v>
       </c>
@@ -4812,7 +4926,7 @@
         <f t="shared" si="8"/>
         <v>54.216882608377716</v>
       </c>
-      <c r="R25" s="23">
+      <c r="R25" s="21">
         <f t="shared" si="9"/>
         <v>156.21688260837772</v>
       </c>
@@ -4865,7 +4979,7 @@
         <f t="shared" si="8"/>
         <v>51.717168934315794</v>
       </c>
-      <c r="R26" s="23">
+      <c r="R26" s="21">
         <f t="shared" si="9"/>
         <v>162.71716893431579</v>
       </c>
@@ -4918,7 +5032,7 @@
         <f t="shared" si="8"/>
         <v>50.804959999998459</v>
       </c>
-      <c r="R27" s="23">
+      <c r="R27" s="21">
         <f t="shared" si="9"/>
         <v>164.80495999999846</v>
       </c>
@@ -4971,7 +5085,7 @@
         <f t="shared" si="8"/>
         <v>51.607232307836966</v>
       </c>
-      <c r="R28" s="23">
+      <c r="R28" s="21">
         <f t="shared" si="9"/>
         <v>160.60723230783697</v>
       </c>
@@ -5024,7 +5138,7 @@
         <f t="shared" si="8"/>
         <v>54.077971929850264</v>
       </c>
-      <c r="R29" s="23">
+      <c r="R29" s="21">
         <f t="shared" si="9"/>
         <v>151.07797192985026</v>
       </c>
@@ -5077,7 +5191,7 @@
         <f t="shared" si="8"/>
         <v>58.020060528607246</v>
       </c>
-      <c r="R30" s="23">
+      <c r="R30" s="21">
         <f t="shared" si="9"/>
         <v>193.02006052860725</v>
       </c>
@@ -5130,7 +5244,7 @@
         <f t="shared" si="8"/>
         <v>63.115446284296468</v>
       </c>
-      <c r="R31" s="23">
+      <c r="R31" s="21">
         <f t="shared" si="9"/>
         <v>261.11544628429647</v>
       </c>
@@ -5183,7 +5297,7 @@
         <f t="shared" si="8"/>
         <v>68.961472656250862</v>
       </c>
-      <c r="R32" s="23">
+      <c r="R32" s="21">
         <f t="shared" si="9"/>
         <v>179.96147265625086</v>
       </c>
@@ -5236,7 +5350,7 @@
         <f t="shared" si="8"/>
         <v>75.111237907696704</v>
       </c>
-      <c r="R33" s="23">
+      <c r="R33" s="21">
         <f t="shared" si="9"/>
         <v>121.1112379076967</v>
       </c>
@@ -5289,7 +5403,7 @@
         <f t="shared" si="8"/>
         <v>81.115858321876658</v>
       </c>
-      <c r="R34" s="23">
+      <c r="R34" s="21">
         <f t="shared" si="9"/>
         <v>81.115858321876658</v>
       </c>
@@ -5342,7 +5456,7 @@
         <f t="shared" si="8"/>
         <v>86.566508038145003</v>
       </c>
-      <c r="R35" s="23">
+      <c r="R35" s="21">
         <f t="shared" si="9"/>
         <v>137.566508038145</v>
       </c>
@@ -5395,7 +5509,7 @@
         <f t="shared" si="8"/>
         <v>91.134108436660426</v>
       </c>
-      <c r="R36" s="23">
+      <c r="R36" s="21">
         <f t="shared" si="9"/>
         <v>142.13410843666043</v>
       </c>
@@ -5448,7 +5562,7 @@
         <f t="shared" si="8"/>
         <v>94.604540000005727</v>
       </c>
-      <c r="R37" s="23">
+      <c r="R37" s="21">
         <f t="shared" si="9"/>
         <v>145.60454000000573</v>
       </c>
@@ -5501,7 +5615,7 @@
         <f t="shared" si="8"/>
         <v>96.907249580173811</v>
       </c>
-      <c r="R38" s="23">
+      <c r="R38" s="21">
         <f t="shared" si="9"/>
         <v>147.90724958017381</v>
       </c>
@@ -5554,7 +5668,7 @@
         <f t="shared" si="8"/>
         <v>98.135125999608135</v>
       </c>
-      <c r="R39" s="23">
+      <c r="R39" s="21">
         <f t="shared" si="9"/>
         <v>149.13512599960814</v>
       </c>
@@ -5607,7 +5721,7 @@
         <f t="shared" si="8"/>
         <v>98.553516914467764</v>
       </c>
-      <c r="R40" s="23">
+      <c r="R40" s="21">
         <f t="shared" si="9"/>
         <v>149.55351691446776</v>
       </c>
@@ -5660,7 +5774,7 @@
         <f t="shared" si="8"/>
         <v>98.596259868900233</v>
       </c>
-      <c r="R41" s="23">
+      <c r="R41" s="21">
         <f t="shared" si="9"/>
         <v>149.59625986890023</v>
       </c>
@@ -5713,7 +5827,7 @@
         <f t="shared" si="8"/>
         <v>98.846600468765246</v>
       </c>
-      <c r="R42" s="23">
+      <c r="R42" s="21">
         <f t="shared" si="9"/>
         <v>149.84660046876525</v>
       </c>
@@ -5766,7 +5880,7 @@
         <f t="shared" si="8"/>
         <v>100.00087060269288</v>
       </c>
-      <c r="R43" s="23">
+      <c r="R43" s="21">
         <f t="shared" si="9"/>
         <v>151.00087060269288</v>
       </c>
@@ -5819,7 +5933,7 @@
         <f t="shared" si="8"/>
         <v>102.81279964051646</v>
       </c>
-      <c r="R44" s="23">
+      <c r="R44" s="21">
         <f t="shared" si="9"/>
         <v>153.81279964051646</v>
       </c>
@@ -5872,7 +5986,7 @@
         <f t="shared" si="8"/>
         <v>108.01633153508737</v>
       </c>
-      <c r="R45" s="23">
+      <c r="R45" s="21">
         <f t="shared" si="9"/>
         <v>159.01633153508737</v>
       </c>
@@ -5925,7 +6039,7 @@
         <f t="shared" si="8"/>
         <v>116.22482075856533</v>
       </c>
-      <c r="R46" s="23">
+      <c r="R46" s="21">
         <f t="shared" si="9"/>
         <v>167.22482075856533</v>
       </c>
@@ -5978,7 +6092,7 @@
         <f t="shared" si="8"/>
         <v>127.80448000003526</v>
       </c>
-      <c r="R47" s="23">
+      <c r="R47" s="21">
         <f t="shared" si="9"/>
         <v>178.80448000003526</v>
       </c>
@@ -6031,7 +6145,7 @@
         <f t="shared" si="8"/>
         <v>142.7199525529868</v>
       </c>
-      <c r="R48" s="23">
+      <c r="R48" s="21">
         <f t="shared" si="9"/>
         <v>193.7199525529868</v>
       </c>
@@ -6084,7 +6198,7 @@
         <f t="shared" si="8"/>
         <v>160.34988232213072</v>
       </c>
-      <c r="R49" s="23">
+      <c r="R49" s="21">
         <f t="shared" si="9"/>
         <v>211.34988232213072</v>
       </c>
@@ -6139,7 +6253,7 @@
         <f t="shared" si="8"/>
         <v>179.27035437755694</v>
       </c>
-      <c r="R50" s="23">
+      <c r="R50" s="21">
         <f t="shared" si="9"/>
         <v>230.27035437755694</v>
       </c>
@@ -6192,7 +6306,7 @@
         <f t="shared" si="8"/>
         <v>197.00407898309641</v>
       </c>
-      <c r="R51" s="23">
+      <c r="R51" s="21">
         <f t="shared" si="9"/>
         <v>248.00407898309641</v>
       </c>
@@ -6245,7 +6359,7 @@
         <f t="shared" si="8"/>
         <v>209.73319203127176</v>
       </c>
-      <c r="R52" s="23">
+      <c r="R52" s="21">
         <f t="shared" si="9"/>
         <v>260.73319203127176</v>
       </c>
@@ -6298,7 +6412,7 @@
         <f t="shared" si="8"/>
         <v>211.97354480810463</v>
       </c>
-      <c r="R53" s="23">
+      <c r="R53" s="21">
         <f t="shared" si="9"/>
         <v>262.97354480810463</v>
       </c>
@@ -6351,7 +6465,7 @@
         <f t="shared" si="8"/>
         <v>196.20835602207808</v>
       </c>
-      <c r="R54" s="23">
+      <c r="R54" s="21">
         <f t="shared" si="9"/>
         <v>247.20835602207808</v>
       </c>
@@ -6404,7 +6518,7 @@
         <f t="shared" si="8"/>
         <v>152.47909901948879</v>
       </c>
-      <c r="R55" s="23">
+      <c r="R55" s="21">
         <f t="shared" si="9"/>
         <v>203.47909901948879</v>
       </c>
@@ -6457,7 +6571,7 @@
         <f t="shared" si="8"/>
         <v>67.93149712018203</v>
       </c>
-      <c r="R56" s="23">
+      <c r="R56" s="21">
         <f t="shared" si="9"/>
         <v>118.93149712018203</v>
       </c>
@@ -6510,7 +6624,7 @@
         <f t="shared" si="8"/>
         <v>-73.685499999963213</v>
       </c>
-      <c r="R57" s="23">
+      <c r="R57" s="21">
         <f t="shared" si="9"/>
         <v>-22.685499999963213</v>
       </c>
@@ -6561,7 +6675,7 @@
         <f t="shared" si="8"/>
         <v>-292.5698859540862</v>
       </c>
-      <c r="R58" s="23">
+      <c r="R58" s="21">
         <f t="shared" si="9"/>
         <v>-292.5698859540862</v>
       </c>
@@ -6635,10 +6749,10 @@
       <c r="G7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="25"/>
+      <c r="I7" s="23"/>
       <c r="J7" s="11" t="s">
         <v>26</v>
       </c>
@@ -6671,7 +6785,7 @@
       </c>
     </row>
     <row r="8" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D8" s="26">
+      <c r="D8" s="24">
         <v>3</v>
       </c>
       <c r="E8" s="7">
@@ -6722,7 +6836,7 @@
         <f>J8+K8+L8+M8+N8+O8+P8</f>
         <v>72.69090358436199</v>
       </c>
-      <c r="R8" s="23">
+      <c r="R8" s="21">
         <f>Q8+F8</f>
         <v>158.69090358436199</v>
       </c>
@@ -6732,7 +6846,7 @@
       </c>
     </row>
     <row r="9" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D9" s="26"/>
+      <c r="D9" s="24"/>
       <c r="E9" s="7" t="s">
         <v>0</v>
       </c>
@@ -6782,7 +6896,7 @@
         <f t="shared" ref="Q9:Q58" si="8">J9+K9+L9+M9+N9+O9+P9</f>
         <v>8.9997716687359777</v>
       </c>
-      <c r="R9" s="23">
+      <c r="R9" s="21">
         <f>Q9+F9</f>
         <v>119.99977166873597</v>
       </c>
@@ -6792,7 +6906,7 @@
       </c>
     </row>
     <row r="10" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D10" s="26"/>
+      <c r="D10" s="24"/>
       <c r="E10" s="7">
         <v>63</v>
       </c>
@@ -6842,7 +6956,7 @@
         <f t="shared" si="8"/>
         <v>-19.513397891506013</v>
       </c>
-      <c r="R10" s="23">
+      <c r="R10" s="21">
         <f t="shared" ref="R10:R58" si="9">Q10+F10</f>
         <v>79.486602108493983</v>
       </c>
@@ -6852,7 +6966,7 @@
       </c>
     </row>
     <row r="11" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D11" s="26"/>
+      <c r="D11" s="24"/>
       <c r="E11" s="7">
         <v>88</v>
       </c>
@@ -6902,7 +7016,7 @@
         <f t="shared" si="8"/>
         <v>-24.765965576192066</v>
       </c>
-      <c r="R11" s="23">
+      <c r="R11" s="21">
         <f t="shared" si="9"/>
         <v>111.23403442380794</v>
       </c>
@@ -6912,7 +7026,7 @@
       </c>
     </row>
     <row r="12" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D12" s="26"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="7">
         <v>73</v>
       </c>
@@ -6962,7 +7076,7 @@
         <f t="shared" si="8"/>
         <v>-15.891621718750054</v>
       </c>
-      <c r="R12" s="23">
+      <c r="R12" s="21">
         <f t="shared" si="9"/>
         <v>99.108378281249941</v>
       </c>
@@ -6972,7 +7086,7 @@
       </c>
     </row>
     <row r="13" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D13" s="26"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="7">
         <v>20</v>
       </c>
@@ -7022,7 +7136,7 @@
         <f t="shared" si="8"/>
         <v>0.31521416883194397</v>
       </c>
-      <c r="R13" s="23">
+      <c r="R13" s="21">
         <f t="shared" si="9"/>
         <v>32.315214168831943</v>
       </c>
@@ -7032,7 +7146,7 @@
       </c>
     </row>
     <row r="14" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D14" s="26"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="7">
         <v>73</v>
       </c>
@@ -7082,7 +7196,7 @@
         <f t="shared" si="8"/>
         <v>18.999439192965934</v>
       </c>
-      <c r="R14" s="23">
+      <c r="R14" s="21">
         <f t="shared" si="9"/>
         <v>133.99943919296592</v>
       </c>
@@ -7141,7 +7255,7 @@
         <f t="shared" si="8"/>
         <v>36.887630925823714</v>
       </c>
-      <c r="R15" s="23">
+      <c r="R15" s="21">
         <f t="shared" si="9"/>
         <v>234.88763092582371</v>
       </c>
@@ -7196,7 +7310,7 @@
         <f t="shared" si="8"/>
         <v>51.970602231577047</v>
       </c>
-      <c r="R16" s="23">
+      <c r="R16" s="21">
         <f t="shared" si="9"/>
         <v>162.97060223157706</v>
       </c>
@@ -7251,7 +7365,7 @@
         <f t="shared" si="8"/>
         <v>63.224019999999804</v>
       </c>
-      <c r="R17" s="23">
+      <c r="R17" s="21">
         <f t="shared" si="9"/>
         <v>95.224019999999797</v>
       </c>
@@ -7306,7 +7420,7 @@
         <f t="shared" si="8"/>
         <v>70.364960715901049</v>
       </c>
-      <c r="R18" s="23">
+      <c r="R18" s="21">
         <f t="shared" si="9"/>
         <v>188.36496071590105</v>
       </c>
@@ -7361,7 +7475,7 @@
         <f t="shared" si="8"/>
         <v>73.642275792896285</v>
       </c>
-      <c r="R19" s="23">
+      <c r="R19" s="21">
         <f t="shared" si="9"/>
         <v>174.64227579289627</v>
       </c>
@@ -7416,7 +7530,7 @@
         <f t="shared" si="8"/>
         <v>73.65863959995248</v>
       </c>
-      <c r="R20" s="23">
+      <c r="R20" s="21">
         <f t="shared" si="9"/>
         <v>183.65863959995249</v>
       </c>
@@ -7471,7 +7585,7 @@
         <f t="shared" si="8"/>
         <v>71.222153109247301</v>
       </c>
-      <c r="R21" s="23">
+      <c r="R21" s="21">
         <f t="shared" si="9"/>
         <v>170.2221531092473</v>
       </c>
@@ -7524,7 +7638,7 @@
         <f t="shared" si="8"/>
         <v>67.225376093749659</v>
       </c>
-      <c r="R22" s="23">
+      <c r="R22" s="21">
         <f t="shared" si="9"/>
         <v>168.22537609374967</v>
       </c>
@@ -7577,7 +7691,7 @@
         <f t="shared" si="8"/>
         <v>62.549660803071276</v>
       </c>
-      <c r="R23" s="23">
+      <c r="R23" s="21">
         <f t="shared" si="9"/>
         <v>162.54966080307128</v>
       </c>
@@ -7630,7 +7744,7 @@
         <f t="shared" si="8"/>
         <v>57.992660046023218</v>
       </c>
-      <c r="R24" s="23">
+      <c r="R24" s="21">
         <f t="shared" si="9"/>
         <v>168.99266004602322</v>
       </c>
@@ -7683,7 +7797,7 @@
         <f t="shared" si="8"/>
         <v>54.216882608377716</v>
       </c>
-      <c r="R25" s="23">
+      <c r="R25" s="21">
         <f t="shared" si="9"/>
         <v>188.21688260837772</v>
       </c>
@@ -7736,7 +7850,7 @@
         <f t="shared" si="8"/>
         <v>51.717168934315794</v>
       </c>
-      <c r="R26" s="23">
+      <c r="R26" s="21">
         <f t="shared" si="9"/>
         <v>165.71716893431579</v>
       </c>
@@ -7789,7 +7903,7 @@
         <f t="shared" si="8"/>
         <v>50.804959999998459</v>
       </c>
-      <c r="R27" s="23">
+      <c r="R27" s="21">
         <f t="shared" si="9"/>
         <v>151.80495999999846</v>
       </c>
@@ -7842,7 +7956,7 @@
         <f t="shared" si="8"/>
         <v>51.607232307836966</v>
       </c>
-      <c r="R28" s="23">
+      <c r="R28" s="21">
         <f t="shared" si="9"/>
         <v>166.60723230783697</v>
       </c>
@@ -7895,7 +8009,7 @@
         <f t="shared" si="8"/>
         <v>54.077971929850264</v>
       </c>
-      <c r="R29" s="23">
+      <c r="R29" s="21">
         <f t="shared" si="9"/>
         <v>98.077971929850264</v>
       </c>
@@ -7948,7 +8062,7 @@
         <f t="shared" si="8"/>
         <v>58.020060528607246</v>
       </c>
-      <c r="R30" s="23">
+      <c r="R30" s="21">
         <f t="shared" si="9"/>
         <v>58.020060528607246</v>
       </c>
@@ -8001,7 +8115,7 @@
         <f t="shared" si="8"/>
         <v>63.115446284296468</v>
       </c>
-      <c r="R31" s="23">
+      <c r="R31" s="21">
         <f t="shared" si="9"/>
         <v>149.11544628429647</v>
       </c>
@@ -8054,7 +8168,7 @@
         <f t="shared" si="8"/>
         <v>68.961472656250862</v>
       </c>
-      <c r="R32" s="23">
+      <c r="R32" s="21">
         <f t="shared" si="9"/>
         <v>179.96147265625086</v>
       </c>
@@ -8107,7 +8221,7 @@
         <f t="shared" si="8"/>
         <v>75.111237907696704</v>
       </c>
-      <c r="R33" s="23">
+      <c r="R33" s="21">
         <f t="shared" si="9"/>
         <v>174.1112379076967</v>
       </c>
@@ -8160,7 +8274,7 @@
         <f t="shared" si="8"/>
         <v>81.115858321876658</v>
       </c>
-      <c r="R34" s="23">
+      <c r="R34" s="21">
         <f t="shared" si="9"/>
         <v>217.11585832187666</v>
       </c>
@@ -8213,7 +8327,7 @@
         <f t="shared" si="8"/>
         <v>86.566508038145003</v>
       </c>
-      <c r="R35" s="23">
+      <c r="R35" s="21">
         <f t="shared" si="9"/>
         <v>201.566508038145</v>
       </c>
@@ -8266,7 +8380,7 @@
         <f t="shared" si="8"/>
         <v>91.134108436660426</v>
       </c>
-      <c r="R36" s="23">
+      <c r="R36" s="21">
         <f t="shared" si="9"/>
         <v>123.13410843666043</v>
       </c>
@@ -8319,7 +8433,7 @@
         <f t="shared" si="8"/>
         <v>94.604540000005727</v>
       </c>
-      <c r="R37" s="23">
+      <c r="R37" s="21">
         <f t="shared" si="9"/>
         <v>209.60454000000573</v>
       </c>
@@ -8372,7 +8486,7 @@
         <f t="shared" si="8"/>
         <v>96.907249580173811</v>
       </c>
-      <c r="R38" s="23">
+      <c r="R38" s="21">
         <f t="shared" si="9"/>
         <v>294.90724958017381</v>
       </c>
@@ -8425,7 +8539,7 @@
         <f t="shared" si="8"/>
         <v>98.135125999608135</v>
       </c>
-      <c r="R39" s="23">
+      <c r="R39" s="21">
         <f t="shared" si="9"/>
         <v>209.13512599960814</v>
       </c>
@@ -8478,7 +8592,7 @@
         <f t="shared" si="8"/>
         <v>98.553516914467764</v>
       </c>
-      <c r="R40" s="23">
+      <c r="R40" s="21">
         <f t="shared" si="9"/>
         <v>130.55351691446776</v>
       </c>
@@ -8531,7 +8645,7 @@
         <f t="shared" si="8"/>
         <v>98.596259868900233</v>
       </c>
-      <c r="R41" s="23">
+      <c r="R41" s="21">
         <f t="shared" si="9"/>
         <v>216.59625986890023</v>
       </c>
@@ -8584,7 +8698,7 @@
         <f t="shared" si="8"/>
         <v>98.846600468765246</v>
       </c>
-      <c r="R42" s="23">
+      <c r="R42" s="21">
         <f t="shared" si="9"/>
         <v>199.84660046876525</v>
       </c>
@@ -8637,7 +8751,7 @@
         <f t="shared" si="8"/>
         <v>100.00087060269288</v>
       </c>
-      <c r="R43" s="23">
+      <c r="R43" s="21">
         <f t="shared" si="9"/>
         <v>210.00087060269288</v>
       </c>
@@ -8690,7 +8804,7 @@
         <f t="shared" si="8"/>
         <v>102.81279964051646</v>
       </c>
-      <c r="R44" s="23">
+      <c r="R44" s="21">
         <f t="shared" si="9"/>
         <v>201.81279964051646</v>
       </c>
@@ -8743,7 +8857,7 @@
         <f t="shared" si="8"/>
         <v>108.01633153508737</v>
       </c>
-      <c r="R45" s="23">
+      <c r="R45" s="21">
         <f t="shared" si="9"/>
         <v>209.01633153508737</v>
       </c>
@@ -8796,7 +8910,7 @@
         <f t="shared" si="8"/>
         <v>116.22482075856533</v>
       </c>
-      <c r="R46" s="23">
+      <c r="R46" s="21">
         <f t="shared" si="9"/>
         <v>216.22482075856533</v>
       </c>
@@ -8849,7 +8963,7 @@
         <f t="shared" si="8"/>
         <v>127.80448000003526</v>
       </c>
-      <c r="R47" s="23">
+      <c r="R47" s="21">
         <f t="shared" si="9"/>
         <v>238.80448000003526</v>
       </c>
@@ -8902,7 +9016,7 @@
         <f t="shared" si="8"/>
         <v>142.7199525529868</v>
       </c>
-      <c r="R48" s="23">
+      <c r="R48" s="21">
         <f t="shared" si="9"/>
         <v>276.7199525529868</v>
       </c>
@@ -8955,7 +9069,7 @@
         <f t="shared" si="8"/>
         <v>160.34988232213072</v>
       </c>
-      <c r="R49" s="23">
+      <c r="R49" s="21">
         <f t="shared" si="9"/>
         <v>274.34988232213072</v>
       </c>
@@ -9010,7 +9124,7 @@
         <f t="shared" si="8"/>
         <v>179.27035437755694</v>
       </c>
-      <c r="R50" s="23">
+      <c r="R50" s="21">
         <f t="shared" si="9"/>
         <v>280.27035437755694</v>
       </c>
@@ -9063,7 +9177,7 @@
         <f t="shared" si="8"/>
         <v>197.00407898309641</v>
       </c>
-      <c r="R51" s="23">
+      <c r="R51" s="21">
         <f t="shared" si="9"/>
         <v>312.00407898309641</v>
       </c>
@@ -9116,7 +9230,7 @@
         <f t="shared" si="8"/>
         <v>209.73319203127176</v>
       </c>
-      <c r="R52" s="23">
+      <c r="R52" s="21">
         <f t="shared" si="9"/>
         <v>253.73319203127176</v>
       </c>
@@ -9169,7 +9283,7 @@
         <f t="shared" si="8"/>
         <v>211.97354480810463</v>
       </c>
-      <c r="R53" s="23">
+      <c r="R53" s="21">
         <f t="shared" si="9"/>
         <v>211.97354480810463</v>
       </c>
@@ -9222,7 +9336,7 @@
         <f t="shared" si="8"/>
         <v>196.20835602207808</v>
       </c>
-      <c r="R54" s="23">
+      <c r="R54" s="21">
         <f t="shared" si="9"/>
         <v>247.20835602207808</v>
       </c>
@@ -9275,7 +9389,7 @@
         <f t="shared" si="8"/>
         <v>152.47909901948879</v>
       </c>
-      <c r="R55" s="23">
+      <c r="R55" s="21">
         <f t="shared" si="9"/>
         <v>196.47909901948879</v>
       </c>
@@ -9328,7 +9442,7 @@
         <f t="shared" si="8"/>
         <v>67.93149712018203</v>
       </c>
-      <c r="R56" s="23">
+      <c r="R56" s="21">
         <f t="shared" si="9"/>
         <v>111.93149712018203</v>
       </c>
@@ -9381,7 +9495,7 @@
         <f t="shared" si="8"/>
         <v>-73.685499999963213</v>
       </c>
-      <c r="R57" s="23">
+      <c r="R57" s="21">
         <f t="shared" si="9"/>
         <v>-29.685499999963213</v>
       </c>
@@ -9432,7 +9546,7 @@
         <f t="shared" si="8"/>
         <v>-292.5698859540862</v>
       </c>
-      <c r="R58" s="23">
+      <c r="R58" s="21">
         <f t="shared" si="9"/>
         <v>-292.5698859540862</v>
       </c>
@@ -9476,8 +9590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBB1CFD0-42E3-417A-AA5C-4D2F28CB3F1B}">
   <dimension ref="D7:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B11" sqref="A11:XFD11"/>
+    <sheetView topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13:S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9511,10 +9625,10 @@
       <c r="G7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="25"/>
+      <c r="I7" s="23"/>
       <c r="J7" s="11" t="s">
         <v>26</v>
       </c>
@@ -9547,7 +9661,7 @@
       </c>
     </row>
     <row r="8" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D8" s="26">
+      <c r="D8" s="24">
         <v>3</v>
       </c>
       <c r="E8" s="7">
@@ -9598,7 +9712,7 @@
         <f>J8+K8+L8+M8+N8+O8+P8</f>
         <v>72.69090358436199</v>
       </c>
-      <c r="R8" s="23">
+      <c r="R8" s="21">
         <f>Q8+F8</f>
         <v>158.69090358436199</v>
       </c>
@@ -9608,7 +9722,7 @@
       </c>
     </row>
     <row r="9" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D9" s="26"/>
+      <c r="D9" s="24"/>
       <c r="E9" s="7" t="s">
         <v>0</v>
       </c>
@@ -9658,7 +9772,7 @@
         <f t="shared" ref="Q9:Q58" si="8">J9+K9+L9+M9+N9+O9+P9</f>
         <v>8.9997716687359777</v>
       </c>
-      <c r="R9" s="23">
+      <c r="R9" s="21">
         <f>Q9+F9</f>
         <v>119.99977166873597</v>
       </c>
@@ -9668,7 +9782,7 @@
       </c>
     </row>
     <row r="10" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D10" s="26"/>
+      <c r="D10" s="24"/>
       <c r="E10" s="7">
         <v>63</v>
       </c>
@@ -9718,7 +9832,7 @@
         <f t="shared" si="8"/>
         <v>-19.513397891506013</v>
       </c>
-      <c r="R10" s="23">
+      <c r="R10" s="21">
         <f t="shared" ref="R10:R58" si="9">Q10+F10</f>
         <v>79.486602108493983</v>
       </c>
@@ -9728,7 +9842,7 @@
       </c>
     </row>
     <row r="11" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D11" s="26"/>
+      <c r="D11" s="24"/>
       <c r="E11" s="7">
         <v>88</v>
       </c>
@@ -9778,7 +9892,7 @@
         <f t="shared" si="8"/>
         <v>-24.765965576192066</v>
       </c>
-      <c r="R11" s="23">
+      <c r="R11" s="21">
         <f t="shared" si="9"/>
         <v>111.23403442380794</v>
       </c>
@@ -9788,7 +9902,7 @@
       </c>
     </row>
     <row r="12" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D12" s="26"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="7">
         <v>73</v>
       </c>
@@ -9838,7 +9952,7 @@
         <f t="shared" si="8"/>
         <v>-15.891621718750054</v>
       </c>
-      <c r="R12" s="23">
+      <c r="R12" s="21">
         <f t="shared" si="9"/>
         <v>99.108378281249941</v>
       </c>
@@ -9848,7 +9962,7 @@
       </c>
     </row>
     <row r="13" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D13" s="26"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="7" t="s">
         <v>4</v>
       </c>
@@ -9898,7 +10012,7 @@
         <f t="shared" si="8"/>
         <v>0.31521416883194397</v>
       </c>
-      <c r="R13" s="23">
+      <c r="R13" s="21">
         <f t="shared" si="9"/>
         <v>195.31521416883194</v>
       </c>
@@ -9908,7 +10022,7 @@
       </c>
     </row>
     <row r="14" spans="4:19" x14ac:dyDescent="0.3">
-      <c r="D14" s="26"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="7">
         <v>20</v>
       </c>
@@ -9958,7 +10072,7 @@
         <f t="shared" si="8"/>
         <v>18.999439192965934</v>
       </c>
-      <c r="R14" s="23">
+      <c r="R14" s="21">
         <f t="shared" si="9"/>
         <v>50.999439192965937</v>
       </c>
@@ -10017,7 +10131,7 @@
         <f t="shared" si="8"/>
         <v>36.887630925823714</v>
       </c>
-      <c r="R15" s="23">
+      <c r="R15" s="21">
         <f t="shared" si="9"/>
         <v>135.88763092582371</v>
       </c>
@@ -10072,7 +10186,7 @@
         <f t="shared" si="8"/>
         <v>51.970602231577047</v>
       </c>
-      <c r="R16" s="23">
+      <c r="R16" s="21">
         <f t="shared" si="9"/>
         <v>162.97060223157706</v>
       </c>
@@ -10127,7 +10241,7 @@
         <f t="shared" si="8"/>
         <v>63.224019999999804</v>
       </c>
-      <c r="R17" s="23">
+      <c r="R17" s="21">
         <f t="shared" si="9"/>
         <v>173.2240199999998</v>
       </c>
@@ -10182,7 +10296,7 @@
         <f t="shared" si="8"/>
         <v>70.364960715901049</v>
       </c>
-      <c r="R18" s="23">
+      <c r="R18" s="21">
         <f t="shared" si="9"/>
         <v>185.36496071590105</v>
       </c>
@@ -10237,7 +10351,7 @@
         <f t="shared" si="8"/>
         <v>73.642275792896285</v>
       </c>
-      <c r="R19" s="23">
+      <c r="R19" s="21">
         <f t="shared" si="9"/>
         <v>174.64227579289627</v>
       </c>
@@ -10292,7 +10406,7 @@
         <f t="shared" si="8"/>
         <v>73.65863959995248</v>
       </c>
-      <c r="R20" s="23">
+      <c r="R20" s="21">
         <f t="shared" si="9"/>
         <v>176.65863959995249</v>
       </c>
@@ -10347,7 +10461,7 @@
         <f t="shared" si="8"/>
         <v>71.222153109247301</v>
       </c>
-      <c r="R21" s="23">
+      <c r="R21" s="21">
         <f t="shared" si="9"/>
         <v>188.2221531092473</v>
       </c>
@@ -10400,7 +10514,7 @@
         <f t="shared" si="8"/>
         <v>67.225376093749659</v>
       </c>
-      <c r="R22" s="23">
+      <c r="R22" s="21">
         <f t="shared" si="9"/>
         <v>168.22537609374967</v>
       </c>
@@ -10453,7 +10567,7 @@
         <f t="shared" si="8"/>
         <v>62.549660803071276</v>
       </c>
-      <c r="R23" s="23">
+      <c r="R23" s="21">
         <f t="shared" si="9"/>
         <v>171.54966080307128</v>
       </c>
@@ -10506,7 +10620,7 @@
         <f t="shared" si="8"/>
         <v>57.992660046023218</v>
       </c>
-      <c r="R24" s="23">
+      <c r="R24" s="21">
         <f t="shared" si="9"/>
         <v>103.99266004602322</v>
       </c>
@@ -10559,7 +10673,7 @@
         <f t="shared" si="8"/>
         <v>54.216882608377716</v>
       </c>
-      <c r="R25" s="23">
+      <c r="R25" s="21">
         <f t="shared" si="9"/>
         <v>54.216882608377716</v>
       </c>
@@ -10612,7 +10726,7 @@
         <f t="shared" si="8"/>
         <v>51.717168934315794</v>
       </c>
-      <c r="R26" s="23">
+      <c r="R26" s="21">
         <f t="shared" si="9"/>
         <v>96.717168934315794</v>
       </c>
@@ -10665,7 +10779,7 @@
         <f t="shared" si="8"/>
         <v>50.804959999998459</v>
       </c>
-      <c r="R27" s="23">
+      <c r="R27" s="21">
         <f t="shared" si="9"/>
         <v>248.80495999999846</v>
       </c>
@@ -10718,7 +10832,7 @@
         <f t="shared" si="8"/>
         <v>51.607232307836966</v>
       </c>
-      <c r="R28" s="23">
+      <c r="R28" s="21">
         <f t="shared" si="9"/>
         <v>252.60723230783697</v>
       </c>
@@ -10771,7 +10885,7 @@
         <f t="shared" si="8"/>
         <v>54.077971929850264</v>
       </c>
-      <c r="R29" s="23">
+      <c r="R29" s="21">
         <f t="shared" si="9"/>
         <v>87.077971929850264</v>
       </c>
@@ -10824,7 +10938,7 @@
         <f t="shared" si="8"/>
         <v>58.020060528607246</v>
       </c>
-      <c r="R30" s="23">
+      <c r="R30" s="21">
         <f t="shared" si="9"/>
         <v>241.02006052860725</v>
       </c>
@@ -10877,7 +10991,7 @@
         <f t="shared" si="8"/>
         <v>63.115446284296468</v>
       </c>
-      <c r="R31" s="23">
+      <c r="R31" s="21">
         <f t="shared" si="9"/>
         <v>247.11544628429647</v>
       </c>
@@ -10930,7 +11044,7 @@
         <f t="shared" si="8"/>
         <v>68.961472656250862</v>
       </c>
-      <c r="R32" s="23">
+      <c r="R32" s="21">
         <f t="shared" si="9"/>
         <v>195.96147265625086</v>
       </c>
@@ -10983,7 +11097,7 @@
         <f t="shared" si="8"/>
         <v>75.111237907696704</v>
       </c>
-      <c r="R33" s="23">
+      <c r="R33" s="21">
         <f t="shared" si="9"/>
         <v>282.1112379076967</v>
       </c>
@@ -11036,7 +11150,7 @@
         <f t="shared" si="8"/>
         <v>81.115858321876658</v>
       </c>
-      <c r="R34" s="23">
+      <c r="R34" s="21">
         <f t="shared" si="9"/>
         <v>167.11585832187666</v>
       </c>
@@ -11089,7 +11203,7 @@
         <f t="shared" si="8"/>
         <v>86.566508038145003</v>
       </c>
-      <c r="R35" s="23">
+      <c r="R35" s="21">
         <f t="shared" si="9"/>
         <v>197.566508038145</v>
       </c>
@@ -11142,7 +11256,7 @@
         <f t="shared" si="8"/>
         <v>91.134108436660426</v>
       </c>
-      <c r="R36" s="23">
+      <c r="R36" s="21">
         <f t="shared" si="9"/>
         <v>190.13410843666043</v>
       </c>
@@ -11195,7 +11309,7 @@
         <f t="shared" si="8"/>
         <v>94.604540000005727</v>
       </c>
-      <c r="R37" s="23">
+      <c r="R37" s="21">
         <f t="shared" si="9"/>
         <v>230.60454000000573</v>
       </c>
@@ -11248,7 +11362,7 @@
         <f t="shared" si="8"/>
         <v>96.907249580173811</v>
       </c>
-      <c r="R38" s="23">
+      <c r="R38" s="21">
         <f t="shared" si="9"/>
         <v>211.90724958017381</v>
       </c>
@@ -11301,7 +11415,7 @@
         <f t="shared" si="8"/>
         <v>98.135125999608135</v>
       </c>
-      <c r="R39" s="23">
+      <c r="R39" s="21">
         <f t="shared" si="9"/>
         <v>293.13512599960814</v>
       </c>
@@ -11354,7 +11468,7 @@
         <f t="shared" si="8"/>
         <v>98.553516914467764</v>
       </c>
-      <c r="R40" s="23">
+      <c r="R40" s="21">
         <f t="shared" si="9"/>
         <v>130.55351691446776</v>
       </c>
@@ -11407,7 +11521,7 @@
         <f t="shared" si="8"/>
         <v>98.596259868900233</v>
       </c>
-      <c r="R41" s="23">
+      <c r="R41" s="21">
         <f t="shared" si="9"/>
         <v>197.59625986890023</v>
       </c>
@@ -11460,7 +11574,7 @@
         <f t="shared" si="8"/>
         <v>98.846600468765246</v>
       </c>
-      <c r="R42" s="23">
+      <c r="R42" s="21">
         <f t="shared" si="9"/>
         <v>209.84660046876525</v>
       </c>
@@ -11513,7 +11627,7 @@
         <f t="shared" si="8"/>
         <v>100.00087060269288</v>
       </c>
-      <c r="R43" s="23">
+      <c r="R43" s="21">
         <f t="shared" si="9"/>
         <v>210.00087060269288</v>
       </c>
@@ -11566,7 +11680,7 @@
         <f t="shared" si="8"/>
         <v>102.81279964051646</v>
       </c>
-      <c r="R44" s="23">
+      <c r="R44" s="21">
         <f t="shared" si="9"/>
         <v>217.81279964051646</v>
       </c>
@@ -11619,7 +11733,7 @@
         <f t="shared" si="8"/>
         <v>108.01633153508737</v>
       </c>
-      <c r="R45" s="23">
+      <c r="R45" s="21">
         <f t="shared" si="9"/>
         <v>209.01633153508737</v>
       </c>
@@ -11672,7 +11786,7 @@
         <f t="shared" si="8"/>
         <v>116.22482075856533</v>
       </c>
-      <c r="R46" s="23">
+      <c r="R46" s="21">
         <f t="shared" si="9"/>
         <v>219.22482075856533</v>
       </c>
@@ -11725,7 +11839,7 @@
         <f t="shared" si="8"/>
         <v>127.80448000003526</v>
       </c>
-      <c r="R47" s="23">
+      <c r="R47" s="21">
         <f t="shared" si="9"/>
         <v>244.80448000003526</v>
       </c>
@@ -11778,7 +11892,7 @@
         <f t="shared" si="8"/>
         <v>142.7199525529868</v>
       </c>
-      <c r="R48" s="23">
+      <c r="R48" s="21">
         <f t="shared" si="9"/>
         <v>243.7199525529868</v>
       </c>
@@ -11831,7 +11945,7 @@
         <f t="shared" si="8"/>
         <v>160.34988232213072</v>
       </c>
-      <c r="R49" s="23">
+      <c r="R49" s="21">
         <f t="shared" si="9"/>
         <v>269.34988232213072</v>
       </c>
@@ -11886,7 +12000,7 @@
         <f t="shared" si="8"/>
         <v>179.27035437755694</v>
       </c>
-      <c r="R50" s="23">
+      <c r="R50" s="21">
         <f t="shared" si="9"/>
         <v>225.27035437755694</v>
       </c>
@@ -11939,7 +12053,7 @@
         <f t="shared" si="8"/>
         <v>197.00407898309641</v>
       </c>
-      <c r="R51" s="23">
+      <c r="R51" s="21">
         <f t="shared" si="9"/>
         <v>197.00407898309641</v>
       </c>
@@ -11992,7 +12106,7 @@
         <f t="shared" si="8"/>
         <v>209.73319203127176</v>
       </c>
-      <c r="R52" s="23">
+      <c r="R52" s="21">
         <f t="shared" si="9"/>
         <v>254.73319203127176</v>
       </c>
@@ -12045,7 +12159,7 @@
         <f t="shared" si="8"/>
         <v>211.97354480810463</v>
       </c>
-      <c r="R53" s="23">
+      <c r="R53" s="21">
         <f t="shared" si="9"/>
         <v>409.97354480810463</v>
       </c>
@@ -12098,7 +12212,7 @@
         <f t="shared" si="8"/>
         <v>196.20835602207808</v>
       </c>
-      <c r="R54" s="23">
+      <c r="R54" s="21">
         <f t="shared" si="9"/>
         <v>397.20835602207808</v>
       </c>
@@ -12151,7 +12265,7 @@
         <f t="shared" si="8"/>
         <v>152.47909901948879</v>
       </c>
-      <c r="R55" s="23">
+      <c r="R55" s="21">
         <f t="shared" si="9"/>
         <v>185.47909901948879</v>
       </c>
@@ -12204,7 +12318,7 @@
         <f t="shared" si="8"/>
         <v>67.93149712018203</v>
       </c>
-      <c r="R56" s="23">
+      <c r="R56" s="21">
         <f t="shared" si="9"/>
         <v>250.93149712018203</v>
       </c>
@@ -12257,7 +12371,7 @@
         <f t="shared" si="8"/>
         <v>-73.685499999963213</v>
       </c>
-      <c r="R57" s="23">
+      <c r="R57" s="21">
         <f t="shared" si="9"/>
         <v>110.31450000003679</v>
       </c>
@@ -12308,7 +12422,7 @@
         <f t="shared" si="8"/>
         <v>-292.5698859540862</v>
       </c>
-      <c r="R58" s="23">
+      <c r="R58" s="21">
         <f t="shared" si="9"/>
         <v>-292.5698859540862</v>
       </c>

</xml_diff>